<commit_message>
updated data a little to work better with palladio. also created a total edges spreadsheet
</commit_message>
<xml_diff>
--- a/palladio/poets_cities (for palladio).xlsx
+++ b/palladio/poets_cities (for palladio).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="poets" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="137">
   <si>
     <t>Melanippides</t>
   </si>
@@ -488,7 +489,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="32">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -521,8 +522,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -530,9 +545,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="32">
+  <cellStyles count="46">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -549,6 +565,13 @@
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -564,6 +587,13 @@
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,7 +864,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -844,16 +874,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="2"/>
+    <col min="4" max="4" width="8.83203125" style="5"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
     <col min="8" max="8" width="23.83203125" customWidth="1"/>
@@ -863,13 +893,13 @@
       <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -886,17 +916,18 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="5">
         <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>84</v>
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>VLOOKUP(F2,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -908,17 +939,18 @@
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5">
         <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>86</v>
+      <c r="E3" s="1" t="str">
+        <f>VLOOKUP(F3,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -930,17 +962,18 @@
       <c r="A4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>86</v>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>VLOOKUP(F4,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -952,17 +985,18 @@
       <c r="A5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>35</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>86</v>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f>VLOOKUP(F5,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -974,17 +1008,18 @@
       <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>35</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>86</v>
+      <c r="E6" s="1" t="str">
+        <f>VLOOKUP(F6,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -996,17 +1031,18 @@
       <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>86</v>
+      <c r="E7" s="1" t="str">
+        <f>VLOOKUP(F7,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1018,17 +1054,18 @@
       <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>86</v>
+      <c r="E8" s="1" t="str">
+        <f>VLOOKUP(F8,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -1040,17 +1077,18 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>84</v>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f>VLOOKUP(F9,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1062,14 +1100,18 @@
       <c r="A10" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="2">
-        <v>2</v>
+      <c r="D10" s="5">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f>VLOOKUP(F10,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1084,17 +1126,18 @@
       <c r="A11" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="5">
         <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="2">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>84</v>
+      <c r="D11" s="5">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f>VLOOKUP(F11,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1106,17 +1149,18 @@
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="5">
         <v>39</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="2">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>86</v>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>VLOOKUP(F12,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -1128,17 +1172,18 @@
       <c r="A13" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="5">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>84</v>
+      <c r="E13" s="1" t="str">
+        <f>VLOOKUP(F13,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1150,17 +1195,18 @@
       <c r="A14" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="2">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>86</v>
+      <c r="D14" s="5">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f>VLOOKUP(F14,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F14">
         <v>3</v>
@@ -1172,17 +1218,18 @@
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>9</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="2">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>86</v>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f>VLOOKUP(F15,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -1194,14 +1241,18 @@
       <c r="A16" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>57</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="5">
         <v>8</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f>VLOOKUP(F16,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1216,17 +1267,18 @@
       <c r="A17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="5">
         <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="5">
         <v>30</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>86</v>
+      <c r="E17" s="1" t="str">
+        <f>VLOOKUP(F17,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1238,17 +1290,18 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>10</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>84</v>
+      <c r="D18" s="5">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f>VLOOKUP(F18,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1260,17 +1313,18 @@
       <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>19</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="5">
         <v>33</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>84</v>
+      <c r="E19" s="1" t="str">
+        <f>VLOOKUP(F19,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1282,17 +1336,18 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="5">
         <v>13</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
+      <c r="E20" s="1" t="str">
+        <f>VLOOKUP(F20,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1304,17 +1359,18 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="5">
         <v>16</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>86</v>
+      <c r="E21" s="1" t="str">
+        <f>VLOOKUP(F21,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -1326,17 +1382,18 @@
       <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="5">
         <v>26</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>84</v>
+      <c r="E22" s="1" t="str">
+        <f>VLOOKUP(F22,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1348,14 +1405,18 @@
       <c r="A23" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>58</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="2">
-        <v>2</v>
+      <c r="D23" s="5">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1" t="str">
+        <f>VLOOKUP(F23,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1367,17 +1428,18 @@
       <c r="A24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <v>4</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="2">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>84</v>
+      <c r="D24" s="5">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="str">
+        <f>VLOOKUP(F24,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1389,17 +1451,18 @@
       <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="5">
         <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="5">
         <v>15</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>84</v>
+      <c r="E25" s="1" t="str">
+        <f>VLOOKUP(F25,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1411,17 +1474,18 @@
       <c r="A26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="5">
         <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="5">
         <v>30</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>86</v>
+      <c r="E26" s="1" t="str">
+        <f>VLOOKUP(F26,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F26">
         <v>3</v>
@@ -1433,14 +1497,18 @@
       <c r="A27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>59</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="2">
-        <v>1</v>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1" t="str">
+        <f>VLOOKUP(F27,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1452,14 +1520,18 @@
       <c r="A28" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="2">
-        <v>2</v>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1" t="str">
+        <f>VLOOKUP(F28,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1471,14 +1543,18 @@
       <c r="A29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="5">
         <v>6</v>
+      </c>
+      <c r="E29" s="1" t="str">
+        <f>VLOOKUP(F29,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1490,14 +1566,18 @@
       <c r="A30" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="2">
-        <v>2</v>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="str">
+        <f>VLOOKUP(F30,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -1509,17 +1589,18 @@
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="5">
         <v>21</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="2">
-        <v>3</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>84</v>
+      <c r="D31" s="5">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="str">
+        <f>VLOOKUP(F31,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1531,14 +1612,18 @@
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="5">
         <v>62</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="5">
         <v>6</v>
+      </c>
+      <c r="E32" s="1" t="str">
+        <f>VLOOKUP(F32,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1550,14 +1635,18 @@
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="5">
         <v>62</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="2">
-        <v>2</v>
+      <c r="D33" s="5">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="str">
+        <f>VLOOKUP(F33,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F33">
         <v>3</v>
@@ -1569,14 +1658,18 @@
       <c r="A34" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="5">
         <v>64</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="2">
-        <v>3</v>
+      <c r="D34" s="5">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="str">
+        <f>VLOOKUP(F34,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1588,17 +1681,18 @@
       <c r="A35" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="5">
         <v>43</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="5">
         <v>19</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>84</v>
+      <c r="E35" s="1" t="str">
+        <f>VLOOKUP(F35,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1610,17 +1704,18 @@
       <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="5">
         <v>43</v>
       </c>
       <c r="C36" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="5">
         <v>30</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>86</v>
+      <c r="E36" s="1" t="str">
+        <f>VLOOKUP(F36,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F36">
         <v>3</v>
@@ -1632,14 +1727,18 @@
       <c r="A37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="5">
         <v>65</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="5">
         <v>39</v>
+      </c>
+      <c r="E37" s="1" t="str">
+        <f>VLOOKUP(F37,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1651,17 +1750,18 @@
       <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="5">
         <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="5">
         <v>32</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>84</v>
+      <c r="E38" s="1" t="str">
+        <f>VLOOKUP(F38,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1673,17 +1773,18 @@
       <c r="A39" t="s">
         <v>62</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="5">
         <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="5">
         <v>30</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>86</v>
+      <c r="E39" s="1" t="str">
+        <f>VLOOKUP(F39,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -1695,14 +1796,18 @@
       <c r="A40" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="5">
         <v>66</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="2">
-        <v>2</v>
+      <c r="D40" s="5">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="str">
+        <f>VLOOKUP(F40,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1714,14 +1819,18 @@
       <c r="A41" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="5">
         <v>67</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="2">
-        <v>2</v>
+      <c r="D41" s="5">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1" t="str">
+        <f>VLOOKUP(F41,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1733,17 +1842,18 @@
       <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="5">
         <v>42</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
-      <c r="D42" s="2">
-        <v>2</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>84</v>
+      <c r="D42" s="5">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1" t="str">
+        <f>VLOOKUP(F42,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1755,17 +1865,18 @@
       <c r="A43" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="5">
         <v>42</v>
       </c>
       <c r="C43" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="5">
         <v>30</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>86</v>
+      <c r="E43" s="1" t="str">
+        <f>VLOOKUP(F43,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -1777,17 +1888,18 @@
       <c r="A44" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="5">
         <v>42</v>
       </c>
       <c r="C44" t="s">
         <v>73</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="5">
         <v>10</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>86</v>
+      <c r="E44" s="1" t="str">
+        <f>VLOOKUP(F44,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F44">
         <v>3</v>
@@ -1799,14 +1911,18 @@
       <c r="A45" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="5">
         <v>68</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="2">
-        <v>2</v>
+      <c r="D45" s="5">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1" t="str">
+        <f>VLOOKUP(F45,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -1818,17 +1934,18 @@
       <c r="A46" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="5">
         <v>12</v>
       </c>
       <c r="C46" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="2">
-        <v>2</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>84</v>
+      <c r="D46" s="5">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="str">
+        <f>VLOOKUP(F46,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1839,14 +1956,18 @@
       <c r="A47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="5">
         <v>69</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="5">
         <v>40</v>
+      </c>
+      <c r="E47" s="1" t="str">
+        <f>VLOOKUP(F47,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -1857,14 +1978,18 @@
       <c r="A48" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="5">
         <v>70</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D48" s="2">
-        <v>2</v>
+      <c r="D48" s="5">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1" t="str">
+        <f>VLOOKUP(F48,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -1875,14 +2000,18 @@
       <c r="A49" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="5">
         <v>71</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="5">
         <v>32</v>
+      </c>
+      <c r="E49" s="1" t="str">
+        <f>VLOOKUP(F49,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -1893,14 +2022,18 @@
       <c r="A50" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="5">
         <v>72</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="5">
         <v>41</v>
+      </c>
+      <c r="E50" s="1" t="str">
+        <f>VLOOKUP(F50,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1911,14 +2044,18 @@
       <c r="A51" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="5">
         <v>55</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="5">
         <v>6</v>
+      </c>
+      <c r="E51" s="1" t="str">
+        <f>VLOOKUP(F51,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -1929,14 +2066,18 @@
       <c r="A52" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="5">
         <v>55</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="2">
-        <v>2</v>
+      <c r="D52" s="5">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="str">
+        <f>VLOOKUP(F52,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F52">
         <v>3</v>
@@ -1947,14 +2088,18 @@
       <c r="A53" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="5">
         <v>73</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="2">
-        <v>2</v>
+      <c r="D53" s="5">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1" t="str">
+        <f>VLOOKUP(F53,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -1965,17 +2110,18 @@
       <c r="A54" t="s">
         <v>21</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="5">
         <v>13</v>
       </c>
       <c r="C54" t="s">
         <v>3</v>
       </c>
-      <c r="D54" s="2">
-        <v>2</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>86</v>
+      <c r="D54" s="5">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1" t="str">
+        <f>VLOOKUP(F54,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -1986,17 +2132,18 @@
       <c r="A55" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="5">
         <v>51</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
-      <c r="D55" s="2">
-        <v>3</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>84</v>
+      <c r="D55" s="5">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="str">
+        <f>VLOOKUP(F55,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2007,17 +2154,18 @@
       <c r="A56" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="5">
         <v>51</v>
       </c>
       <c r="C56" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="5">
         <v>30</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>86</v>
+      <c r="E56" s="1" t="str">
+        <f>VLOOKUP(F56,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F56">
         <v>3</v>
@@ -2028,17 +2176,18 @@
       <c r="A57" t="s">
         <v>70</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="5">
         <v>51</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
       </c>
-      <c r="D57" s="2">
-        <v>2</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>86</v>
+      <c r="D57" s="5">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1" t="str">
+        <f>VLOOKUP(F57,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -2049,17 +2198,18 @@
       <c r="A58" t="s">
         <v>22</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="5">
         <v>14</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="2">
-        <v>2</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>84</v>
+      <c r="D58" s="5">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1" t="str">
+        <f>VLOOKUP(F58,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2070,14 +2220,18 @@
       <c r="A59" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="5">
         <v>75</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="5">
         <v>10</v>
+      </c>
+      <c r="E59" s="1" t="str">
+        <f>VLOOKUP(F59,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2091,14 +2245,18 @@
       <c r="A60" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="5">
         <v>76</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="5">
         <v>15</v>
+      </c>
+      <c r="E60" s="1" t="str">
+        <f>VLOOKUP(F60,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2109,17 +2267,18 @@
       <c r="A61" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="5">
         <v>46</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="2">
-        <v>2</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>84</v>
+      <c r="D61" s="5">
+        <v>2</v>
+      </c>
+      <c r="E61" s="1" t="str">
+        <f>VLOOKUP(F61,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2130,17 +2289,18 @@
       <c r="A62" t="s">
         <v>29</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="5">
         <v>20</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="5">
         <v>34</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>84</v>
+      <c r="E62" s="1" t="str">
+        <f>VLOOKUP(F62,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2151,17 +2311,18 @@
       <c r="A63" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="5">
         <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="5">
         <v>33</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>86</v>
+      <c r="E63" s="1" t="str">
+        <f>VLOOKUP(F63,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F63">
         <v>3</v>
@@ -2172,17 +2333,18 @@
       <c r="A64" t="s">
         <v>66</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="5">
         <v>47</v>
       </c>
       <c r="C64" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="5">
         <v>31</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>84</v>
+      <c r="E64" s="1" t="str">
+        <f>VLOOKUP(F64,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2194,17 +2356,18 @@
       <c r="A65" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="5">
         <v>47</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="2">
-        <v>2</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>86</v>
+      <c r="D65" s="5">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1" t="str">
+        <f>VLOOKUP(F65,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F65">
         <v>3</v>
@@ -2215,17 +2378,18 @@
       <c r="A66" t="s">
         <v>43</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="5">
         <v>28</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="5">
         <v>9</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>84</v>
+      <c r="E66" s="1" t="str">
+        <f>VLOOKUP(F66,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2237,17 +2401,18 @@
       <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="5">
         <v>3</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="5">
         <v>6</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>84</v>
+      <c r="E67" s="1" t="str">
+        <f>VLOOKUP(F67,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2258,17 +2423,18 @@
       <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="5">
         <v>3</v>
       </c>
       <c r="C68" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="5">
         <v>7</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>86</v>
+      <c r="E68" s="1" t="str">
+        <f>VLOOKUP(F68,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F68">
         <v>3</v>
@@ -2279,17 +2445,18 @@
       <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="5">
         <v>3</v>
       </c>
       <c r="C69" t="s">
         <v>3</v>
       </c>
-      <c r="D69" s="2">
-        <v>2</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>86</v>
+      <c r="D69" s="5">
+        <v>2</v>
+      </c>
+      <c r="E69" s="1" t="str">
+        <f>VLOOKUP(F69,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F69">
         <v>3</v>
@@ -2301,14 +2468,18 @@
       <c r="A70" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="5">
         <v>52</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="5">
         <v>36</v>
+      </c>
+      <c r="E70" s="1" t="str">
+        <f>VLOOKUP(F70,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2319,14 +2490,18 @@
       <c r="A71" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="5">
         <v>52</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="5">
         <v>43</v>
+      </c>
+      <c r="E71" s="1" t="str">
+        <f>VLOOKUP(F71,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F71">
         <v>3</v>
@@ -2338,14 +2513,18 @@
       <c r="A72" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="5">
         <v>52</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="5">
         <v>44</v>
+      </c>
+      <c r="E72" s="1" t="str">
+        <f>VLOOKUP(F72,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F72">
         <v>3</v>
@@ -2356,18 +2535,19 @@
       <c r="A73" t="s">
         <v>0</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="5">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="2">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>84</v>
+      <c r="D73" s="5">
+        <v>1</v>
+      </c>
+      <c r="E73" s="1" t="str">
+        <f>VLOOKUP(F73,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2380,18 +2560,19 @@
       <c r="A74" t="s">
         <v>0</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="5">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="C74" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="5">
         <v>33</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>85</v>
+      <c r="E74" s="1" t="str">
+        <f>VLOOKUP(F74,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>died</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -2403,18 +2584,19 @@
       <c r="A75" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="5">
         <f>1</f>
         <v>1</v>
       </c>
       <c r="C75" t="s">
         <v>3</v>
       </c>
-      <c r="D75" s="2">
-        <v>2</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>86</v>
+      <c r="D75" s="5">
+        <v>2</v>
+      </c>
+      <c r="E75" s="1" t="str">
+        <f>VLOOKUP(F75,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F75">
         <v>3</v>
@@ -2427,14 +2609,18 @@
       <c r="A76" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="5">
         <v>91</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D76" s="5">
-        <v>2</v>
+      <c r="D76" s="6">
+        <v>2</v>
+      </c>
+      <c r="E76" s="1" t="str">
+        <f>VLOOKUP(F76,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2446,17 +2632,18 @@
       <c r="A77" t="s">
         <v>68</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="5">
         <v>48</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
       </c>
-      <c r="D77" s="2">
-        <v>2</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>84</v>
+      <c r="D77" s="5">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1" t="str">
+        <f>VLOOKUP(F77,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -2468,14 +2655,18 @@
       <c r="A78" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="5">
         <v>53</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D78" s="2">
-        <v>2</v>
+      <c r="D78" s="5">
+        <v>2</v>
+      </c>
+      <c r="E78" s="1" t="str">
+        <f>VLOOKUP(F78,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -2489,17 +2680,18 @@
       <c r="A79" t="s">
         <v>69</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="5">
         <v>49</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="2">
-        <v>2</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>86</v>
+      <c r="D79" s="5">
+        <v>2</v>
+      </c>
+      <c r="E79" s="1" t="str">
+        <f>VLOOKUP(F79,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F79">
         <v>3</v>
@@ -2510,17 +2702,18 @@
       <c r="A80" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="5">
         <v>49</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="5">
         <v>30</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>86</v>
+      <c r="E80" s="1" t="str">
+        <f>VLOOKUP(F80,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F80">
         <v>3</v>
@@ -2531,17 +2724,18 @@
       <c r="A81" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="5">
         <v>15</v>
       </c>
       <c r="C81" t="s">
         <v>3</v>
       </c>
-      <c r="D81" s="2">
-        <v>2</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>86</v>
+      <c r="D81" s="5">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1" t="str">
+        <f>VLOOKUP(F81,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F81">
         <v>3</v>
@@ -2552,17 +2746,18 @@
       <c r="A82" t="s">
         <v>24</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="5">
         <v>16</v>
       </c>
       <c r="C82" t="s">
         <v>3</v>
       </c>
-      <c r="D82" s="2">
-        <v>2</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>86</v>
+      <c r="D82" s="5">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1" t="str">
+        <f>VLOOKUP(F82,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F82">
         <v>3</v>
@@ -2574,17 +2769,18 @@
       <c r="A83" t="s">
         <v>44</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="5">
         <v>29</v>
       </c>
       <c r="C83" t="s">
         <v>3</v>
       </c>
-      <c r="D83" s="2">
-        <v>2</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>86</v>
+      <c r="D83" s="5">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="str">
+        <f>VLOOKUP(F83,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F83">
         <v>3</v>
@@ -2595,10 +2791,14 @@
       <c r="A84" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="5">
         <v>78</v>
       </c>
       <c r="C84" s="3"/>
+      <c r="E84" s="1" t="str">
+        <f>VLOOKUP(F84,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
+      </c>
       <c r="F84">
         <v>1</v>
       </c>
@@ -2612,17 +2812,18 @@
       <c r="A85" t="s">
         <v>25</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="5">
         <v>17</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
       </c>
-      <c r="D85" s="2">
-        <v>2</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>86</v>
+      <c r="D85" s="5">
+        <v>2</v>
+      </c>
+      <c r="E85" s="1" t="str">
+        <f>VLOOKUP(F85,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F85">
         <v>3</v>
@@ -2633,14 +2834,18 @@
       <c r="A86" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="5">
         <v>89</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D86" s="2">
-        <v>2</v>
+      <c r="D86" s="5">
+        <v>2</v>
+      </c>
+      <c r="E86" s="1" t="str">
+        <f>VLOOKUP(F86,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -2652,17 +2857,18 @@
       <c r="A87" t="s">
         <v>34</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="5">
         <v>24</v>
       </c>
       <c r="C87" t="s">
         <v>35</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="5">
         <v>35</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>84</v>
+      <c r="E87" s="1" t="str">
+        <f>VLOOKUP(F87,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -2672,17 +2878,18 @@
       <c r="A88" t="s">
         <v>34</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="5">
         <v>24</v>
       </c>
       <c r="C88" t="s">
         <v>36</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="5">
         <v>11</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>85</v>
+      <c r="E88" s="1" t="str">
+        <f>VLOOKUP(F88,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>died</v>
       </c>
       <c r="F88">
         <v>2</v>
@@ -2692,17 +2899,18 @@
       <c r="A89" t="s">
         <v>34</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="5">
         <v>24</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
       </c>
-      <c r="D89" s="2">
-        <v>2</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>86</v>
+      <c r="D89" s="5">
+        <v>2</v>
+      </c>
+      <c r="E89" s="1" t="str">
+        <f>VLOOKUP(F89,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F89">
         <v>3</v>
@@ -2712,17 +2920,18 @@
       <c r="A90" t="s">
         <v>34</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="5">
         <v>24</v>
       </c>
       <c r="C90" t="s">
         <v>76</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="5">
         <v>18</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>86</v>
+      <c r="E90" s="1" t="str">
+        <f>VLOOKUP(F90,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F90">
         <v>3</v>
@@ -2732,17 +2941,18 @@
       <c r="A91" t="s">
         <v>34</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="5">
         <v>24</v>
       </c>
       <c r="C91" t="s">
         <v>61</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="5">
         <v>19</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>86</v>
+      <c r="E91" s="1" t="str">
+        <f>VLOOKUP(F91,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F91">
         <v>3</v>
@@ -2752,17 +2962,18 @@
       <c r="A92" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="5">
         <v>24</v>
       </c>
       <c r="C92" t="s">
         <v>77</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="5">
         <v>20</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>86</v>
+      <c r="E92" s="1" t="str">
+        <f>VLOOKUP(F92,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F92">
         <v>3</v>
@@ -2772,17 +2983,18 @@
       <c r="A93" t="s">
         <v>37</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="5">
         <v>25</v>
       </c>
       <c r="C93" t="s">
         <v>38</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="5">
         <v>21</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>84</v>
+      <c r="E93" s="1" t="str">
+        <f>VLOOKUP(F93,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2792,17 +3004,18 @@
       <c r="A94" t="s">
         <v>9</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="5">
         <v>5</v>
       </c>
       <c r="C94" t="s">
         <v>10</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="5">
         <v>8</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>84</v>
+      <c r="E94" s="1" t="str">
+        <f>VLOOKUP(F94,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -2812,17 +3025,18 @@
       <c r="A95" t="s">
         <v>9</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="5">
         <v>5</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
       </c>
-      <c r="D95" s="2">
-        <v>2</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>86</v>
+      <c r="D95" s="5">
+        <v>2</v>
+      </c>
+      <c r="E95" s="1" t="str">
+        <f>VLOOKUP(F95,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -2832,14 +3046,18 @@
       <c r="A96" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="5">
         <v>82</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D96" s="2">
-        <v>3</v>
+      <c r="D96" s="5">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1" t="str">
+        <f>VLOOKUP(F96,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -2849,17 +3067,18 @@
       <c r="A97" t="s">
         <v>39</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="5">
         <v>26</v>
       </c>
       <c r="C97" t="s">
         <v>40</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="5">
         <v>22</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>84</v>
+      <c r="E97" s="1" t="str">
+        <f>VLOOKUP(F97,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -2869,17 +3088,18 @@
       <c r="A98" t="s">
         <v>39</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="5">
         <v>26</v>
       </c>
       <c r="C98" t="s">
         <v>3</v>
       </c>
-      <c r="D98" s="2">
-        <v>2</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>86</v>
+      <c r="D98" s="5">
+        <v>2</v>
+      </c>
+      <c r="E98" s="1" t="str">
+        <f>VLOOKUP(F98,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F98">
         <v>3</v>
@@ -2889,14 +3109,18 @@
       <c r="A99" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="5">
         <v>83</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="5">
         <v>13</v>
+      </c>
+      <c r="E99" s="1" t="str">
+        <f>VLOOKUP(F99,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -2906,17 +3130,18 @@
       <c r="A100" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="5">
         <v>2</v>
       </c>
       <c r="C100" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="2">
-        <v>3</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>84</v>
+      <c r="D100" s="5">
+        <v>3</v>
+      </c>
+      <c r="E100" s="1" t="str">
+        <f>VLOOKUP(F100,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -2926,17 +3151,18 @@
       <c r="A101" t="s">
         <v>4</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="5">
         <v>2</v>
       </c>
       <c r="C101" t="s">
         <v>49</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="5">
         <v>4</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>86</v>
+      <c r="E101" s="1" t="str">
+        <f>VLOOKUP(F101,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F101">
         <v>3</v>
@@ -2946,17 +3172,18 @@
       <c r="A102" t="s">
         <v>4</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="5">
         <v>2</v>
       </c>
       <c r="C102" t="s">
         <v>27</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="5">
         <v>5</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>86</v>
+      <c r="E102" s="1" t="str">
+        <f>VLOOKUP(F102,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F102">
         <v>3</v>
@@ -2966,17 +3193,18 @@
       <c r="A103" t="s">
         <v>4</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="5">
         <v>2</v>
       </c>
       <c r="C103" t="s">
         <v>3</v>
       </c>
-      <c r="D103" s="2">
-        <v>2</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>86</v>
+      <c r="D103" s="5">
+        <v>2</v>
+      </c>
+      <c r="E103" s="1" t="str">
+        <f>VLOOKUP(F103,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F103">
         <v>3</v>
@@ -2986,14 +3214,18 @@
       <c r="A104" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="5">
         <v>84</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104" s="5">
         <v>42</v>
+      </c>
+      <c r="E104" s="1" t="str">
+        <f>VLOOKUP(F104,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3003,14 +3235,18 @@
       <c r="A105" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="5">
         <v>85</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D105" s="2">
-        <v>2</v>
+      <c r="D105" s="5">
+        <v>2</v>
+      </c>
+      <c r="E105" s="1" t="str">
+        <f>VLOOKUP(F105,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3020,14 +3256,18 @@
       <c r="A106" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="5">
         <v>86</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106" s="5">
         <v>41</v>
+      </c>
+      <c r="E106" s="1" t="str">
+        <f>VLOOKUP(F106,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3037,14 +3277,18 @@
       <c r="A107" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="5">
         <v>54</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107" s="5">
         <v>38</v>
+      </c>
+      <c r="E107" s="1" t="str">
+        <f>VLOOKUP(F107,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3054,17 +3298,18 @@
       <c r="A108" t="s">
         <v>13</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="5">
         <v>7</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108" s="5">
         <v>12</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>84</v>
+      <c r="E108" s="1" t="str">
+        <f>VLOOKUP(F108,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -3074,17 +3319,18 @@
       <c r="A109" t="s">
         <v>13</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="5">
         <v>7</v>
       </c>
       <c r="C109" t="s">
         <v>3</v>
       </c>
-      <c r="D109" s="2">
-        <v>2</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>86</v>
+      <c r="D109" s="5">
+        <v>2</v>
+      </c>
+      <c r="E109" s="1" t="str">
+        <f>VLOOKUP(F109,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F109">
         <v>3</v>
@@ -3094,17 +3340,18 @@
       <c r="A110" t="s">
         <v>13</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="5">
         <v>7</v>
       </c>
       <c r="C110" t="s">
         <v>33</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D110" s="5">
         <v>13</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>86</v>
+      <c r="E110" s="1" t="str">
+        <f>VLOOKUP(F110,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F110">
         <v>3</v>
@@ -3114,17 +3361,18 @@
       <c r="A111" t="s">
         <v>13</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="5">
         <v>7</v>
       </c>
       <c r="C111" t="s">
         <v>74</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111" s="5">
         <v>14</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>86</v>
+      <c r="E111" s="1" t="str">
+        <f>VLOOKUP(F111,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F111">
         <v>3</v>
@@ -3134,17 +3382,18 @@
       <c r="A112" t="s">
         <v>13</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="5">
         <v>7</v>
       </c>
       <c r="C112" t="s">
         <v>42</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112" s="5">
         <v>15</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>86</v>
+      <c r="E112" s="1" t="str">
+        <f>VLOOKUP(F112,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F112">
         <v>3</v>
@@ -3154,17 +3403,18 @@
       <c r="A113" t="s">
         <v>32</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="5">
         <v>22</v>
       </c>
       <c r="C113" t="s">
         <v>75</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113" s="5">
         <v>17</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>84</v>
+      <c r="E113" s="1" t="str">
+        <f>VLOOKUP(F113,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -3174,14 +3424,18 @@
       <c r="A114" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="5">
         <v>87</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114" s="5">
         <v>14</v>
+      </c>
+      <c r="E114" s="1" t="str">
+        <f>VLOOKUP(F114,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -3191,17 +3445,18 @@
       <c r="A115" t="s">
         <v>64</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="5">
         <v>45</v>
       </c>
       <c r="C115" t="s">
         <v>5</v>
       </c>
-      <c r="D115" s="2">
-        <v>3</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>84</v>
+      <c r="D115" s="5">
+        <v>3</v>
+      </c>
+      <c r="E115" s="1" t="str">
+        <f>VLOOKUP(F115,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -3211,17 +3466,18 @@
       <c r="A116" t="s">
         <v>64</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="5">
         <v>45</v>
       </c>
       <c r="C116" t="s">
         <v>56</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116" s="5">
         <v>30</v>
       </c>
-      <c r="E116" s="1" t="s">
-        <v>86</v>
+      <c r="E116" s="1" t="str">
+        <f>VLOOKUP(F116,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F116">
         <v>3</v>
@@ -3231,17 +3487,18 @@
       <c r="A117" t="s">
         <v>11</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="5">
         <v>6</v>
       </c>
       <c r="C117" t="s">
         <v>12</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117" s="5">
         <v>9</v>
       </c>
-      <c r="E117" s="1" t="s">
-        <v>84</v>
+      <c r="E117" s="1" t="str">
+        <f>VLOOKUP(F117,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>born</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -3251,17 +3508,18 @@
       <c r="A118" t="s">
         <v>11</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118" s="5">
         <v>6</v>
       </c>
       <c r="C118" t="s">
         <v>2</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D118" s="5">
         <v>33</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>85</v>
+      <c r="E118" s="1" t="str">
+        <f>VLOOKUP(F118,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>died</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -3271,17 +3529,18 @@
       <c r="A119" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="5">
         <v>6</v>
       </c>
       <c r="C119" t="s">
         <v>3</v>
       </c>
-      <c r="D119" s="2">
-        <v>2</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>86</v>
+      <c r="D119" s="5">
+        <v>2</v>
+      </c>
+      <c r="E119" s="1" t="str">
+        <f>VLOOKUP(F119,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F119">
         <v>3</v>
@@ -3291,17 +3550,18 @@
       <c r="A120" t="s">
         <v>11</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="5">
         <v>6</v>
       </c>
       <c r="C120" t="s">
         <v>73</v>
       </c>
-      <c r="D120" s="2">
+      <c r="D120" s="5">
         <v>10</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>86</v>
+      <c r="E120" s="1" t="str">
+        <f>VLOOKUP(F120,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F120">
         <v>3</v>
@@ -3311,17 +3571,18 @@
       <c r="A121" t="s">
         <v>11</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="5">
         <v>6</v>
       </c>
       <c r="C121" t="s">
         <v>36</v>
       </c>
-      <c r="D121" s="2">
+      <c r="D121" s="5">
         <v>11</v>
       </c>
-      <c r="E121" s="1" t="s">
-        <v>86</v>
+      <c r="E121" s="1" t="str">
+        <f>VLOOKUP(F121,Sheet2!$A$1:$B$3,2,FALSE)</f>
+        <v>performed</v>
       </c>
       <c r="F121">
         <v>3</v>
@@ -3484,4 +3745,48 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>